<commit_message>
prueba 01 junior taladro
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -5,23 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime Diaz\Desktop\pantillas mini-Ecomerce\E-Plaza.com\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\PROYECTO E-PLAZA NO TOCAR\E-Plaza.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAB9EBE-6FAD-47D4-A70D-D489DA359A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BCCBFE-4477-4CA0-B0FC-024634C95079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="productos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>image</t>
   </si>
@@ -213,6 +212,54 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>edward quevedo</t>
+  </si>
+  <si>
+    <t>Taladro Inalambrico</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>130.000</t>
+  </si>
+  <si>
+    <t>Taladro Inalámbrico 21 Voltios, Percutor Con 2 Baterías, Copas, Puntas Y Extensión</t>
+  </si>
+  <si>
+    <t>3224336215</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczObtmbU_tsVak1pMSlQuN4-4Onz8TKrQnKBd-dycgx41VHwpHSVWG2njJT7U9vEMJejJa1fdxxmZc7CAuM4pVHM37jFFDfRJchHoHvxUA3iQGsdSAIgmfdNFRoLJsJjMa-xkMW_15cmerYDk3qJjnt-5g=w475-h633-s-no-gm?authuser=0</t>
   </si>
 </sst>
 </file>
@@ -310,7 +357,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,13 +979,88 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D12" s="7"/>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F21" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subida  de productos prueba 2 junior
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\PROYECTO E-PLAZA NO TOCAR\E-Plaza.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BCCBFE-4477-4CA0-B0FC-024634C95079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2E7FA0-D2AD-47B2-9C9F-6CA1431CB742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="98">
   <si>
     <t>image</t>
   </si>
@@ -260,6 +260,60 @@
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/pw/AP1GczObtmbU_tsVak1pMSlQuN4-4Onz8TKrQnKBd-dycgx41VHwpHSVWG2njJT7U9vEMJejJa1fdxxmZc7CAuM4pVHM37jFFDfRJchHoHvxUA3iQGsdSAIgmfdNFRoLJsJjMa-xkMW_15cmerYDk3qJjnt-5g=w475-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Gimnasia Pasiva</t>
+  </si>
+  <si>
+    <t>Gimnasia Pasiva 8 Electrodos De Pila Y Conectar</t>
+  </si>
+  <si>
+    <t>3224336216</t>
+  </si>
+  <si>
+    <t>Cepillo Secador 3 En 1</t>
+  </si>
+  <si>
+    <t>Cepillo Secador 3 En 1, Cepilla, Seca, Alisa</t>
+  </si>
+  <si>
+    <t>50.000</t>
+  </si>
+  <si>
+    <t>45.000</t>
+  </si>
+  <si>
+    <t>3224336217</t>
+  </si>
+  <si>
+    <t>Combo Gamer</t>
+  </si>
+  <si>
+    <t>Combo Gamer Negro RGB Teclado Y Mouse</t>
+  </si>
+  <si>
+    <t>60.000</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczP43uebQ4gDcWJLejZ7DTWX7sZ1Kve4EdQrf0dyDoz8BzIA7IsnM5TN7OgnN22XYm2PT-aUoxdHoaRZ2-00U0kqfhlR0StybFhWteZQGGkSdI0wgvSpFW-z2t1JsDtX7kG-cA8EwjoiI-gEDucMDlBo1A=w500-h309-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNyOyhYX-cmhTtPph9TaYAmzjNUy75kzfsl_jWyZkOGS0C6TTJBQkx06Yv_3EOMmDj4ULQMr4bSM7_pqkXA0QINGouykld9Mx_Zsl7JOg1ml9g98oquSmlvGknceIZkh7R0TOoBa3BE0CdMZ2unjkNBbg=w432-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNFTrSqJt6NsTEkkAtGM5vvJBbjHyai9N2pi42AVY88GnQ-gHyQKoT-iHh8y2TaQ8qlEaRpzYqYKKYaJIZBfb1kK18W2URs7xJ5_NrKYx7bKhZsN1ufh6oSjdFIKGpH2iFf5M6gYlqPYd0Tp3H-PdqF3g=w500-h489-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNDxVXm5qR802junRd2lyek41EuaONp19hqhF-CFq63rMIKmLkP025CNuWiJNgG6_2NTV8PuN-CO2df_Blvj2bNjNlnQn1fJLX-m4xEtq_Bc3vPmu0vtRUSawxRt-hxgV6lr5UFs10Uv9C8Ixt8ma4ibA=w500-h363-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMThvkBf7W_2DmcdJ0jzASx1GAhBztiFTBvJLHfKAoy2BpG_OoKs1l6RutqtzUR1AslF75pguaxp2eH7tFYlPZflsQXk88FU6o7dUCLuO4Ke1BzOW7t-NVe9t5I7CQj4tYv_CBuiu5ni_24BxQTOxOAug=w500-h428-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMFGpnhAYcuxekUHmsBMgL0NoSjeqF2TIBV6-rOwBHYmvl6pKbsd89tg8Nm6_TTvwBVSSETC1Kb5DODQHHIQnyjXt2N06ar8XQng1lftI0gy_97zK34Koem9FuO6UfAuX59BdtGCPftVmY7d0q862ibIg=w794-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczN_YeDAx1aukAWLluS_995Z9heN-qKegOKTLNuPHJMEBQG-qqL7P4AaQtYt8OwUOXlPuRX1PvM1hiZnGCK3hJQkbedX-ycwIxj8mx5KRjVvYlwTFQ8RnVYrNChSOLxJ8bue909bF0WKzI2Skwf3LsstnA=w600-h600-s-no-gm?authuser=0</t>
   </si>
 </sst>
 </file>
@@ -666,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,20 +1066,100 @@
       <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="F13" s="4"/>
+      <c r="B13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">

</xml_diff>

<commit_message>
agrege mas productos con la tienda importa2 //junior
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\PROYECTO E-PLAZA NO TOCAR\E-Plaza.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A03E3D3-693A-4891-9E23-E4A200F37600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F1CE5E-1899-48B1-A6B3-3C4545EA1264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="151">
   <si>
     <t>image</t>
   </si>
@@ -268,9 +268,6 @@
     <t>Gimnasia Pasiva 8 Electrodos De Pila Y Conectar</t>
   </si>
   <si>
-    <t>3224336216</t>
-  </si>
-  <si>
     <t>Cepillo Secador 3 En 1</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>45.000</t>
   </si>
   <si>
-    <t>3224336217</t>
-  </si>
-  <si>
     <t>Combo Gamer</t>
   </si>
   <si>
@@ -314,13 +308,216 @@
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/pw/AP1GczN_YeDAx1aukAWLluS_995Z9heN-qKegOKTLNuPHJMEBQG-qqL7P4AaQtYt8OwUOXlPuRX1PvM1hiZnGCK3hJQkbedX-ycwIxj8mx5KRjVvYlwTFQ8RnVYrNChSOLxJ8bue909bF0WKzI2Skwf3LsstnA=w600-h600-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Equipo de ejercicio multifuncional: el ejercitador de kegel puede ejercitar completamente los músculos de la parte interna de los muslos, eliminar grasa en las piernas, tonificar los músculos de la parte inferior del disco y hacer que el glúteo sea más tonificado. Al mismo tiempo, es adecuado para practicar varios movimientos de diferentes partes. Es un equipo deportivo ideal.
+Diseño ergonómico: este entrenador de cadera está diseñado con un panel táctil ajustable de 360° para adaptarse mejor a la forma de la pierna y al ángulo de movimiento, su diseño de resorte con fuerte elasticidad y presión te permite ir en cualquier momento y en cualquier lugar. Puedes usarlo para mantenerte saludable.
+Material de alta calidad: el entrenador de cadera para mujer está hecho de material PP y TPE, que no solo es antideslizante, sino que también tiene un mejor tacto. El resorte integrado hace que sea elástico y duradero, y la estructura triangular hace que el muslo sea estable y no se deslice durante el ejercicio, y el efecto de ejercicio es más significativo.
+Fácil de usar: entrenador Kegel, 2-3 series de entrenamiento al día, insiste en hacer ejercicio durante 10 minutos por la mañana y por la noche, concéntrate en los músculos de los muslos, reduce la grasa del muslo, el uso a largo plazo puede mejorar la resistencia física
+Personas aplicables: el entrenador de muslos es adecuado para madres posparto, personas con glúteos planos y trabajo sedentario.
+Puede dar forma a la curva perfecta de glúteos sin hacer dieta, cambiar la postura sedentaria y embellecer la forma de la pierna. Es casi adecuado para cualquier persona que quiera hacer deporte. Las personas que hacen ejercicio o pierden peso, ya sea sentadas en una silla para trabajar o mirar televisión, pueden ejercitar los músculos de los muslos y lograr ejercicio fácil.</t>
+  </si>
+  <si>
+    <t>Ejercitador Pélvico</t>
+  </si>
+  <si>
+    <t>Estufa Eléctrica</t>
+  </si>
+  <si>
+    <t>Estufa Eléctrica 1 puesto Fogón Portátil con exterior de hierro reforzado y quemadores fabricados en acero inoxidable duradero. Cuenta con control de termostato y es fácil de limpiar. Ideal para calentar el carbón y tiene luz de funcionamiento.
+Características:
+Potencia: 1000w
+Voltaje nominal: 110V
+Frecuencia nominal: 50-60hz
+Peso: 597g
+Medidas: Alto 5cm Ancho 22cm Largo 22cm
+Contenido del paquete:
+1 Fogón eléctrico
+Este producto cuenta con termostato para ahorro de energía. Recuerda que la vida útil de tu producto depende directamente de su uso. Te recomendamos seguir todas las instrucciones que trae cada artículo al pie de la letra.</t>
+  </si>
+  <si>
+    <t>Molino de Aluminio</t>
+  </si>
+  <si>
+    <t>74.000</t>
+  </si>
+  <si>
+    <t>Características:
+1. Es adecuado para carne de cerdo picada, carne de res, cordero, pollo, especias, pimienta y salchichas.
+2. Estructura Simple y apariencia novedosa, un gran ayudante cuando haciendo salchicha y albóndigas.
+3. Fácil de operar, montar y limpiar, el rectificado es suave, seguro y confiable.
+4. Diseño ergonómico del mango de la manivela, mango súper largo, agarre cómodo, más ahorro de trabajo, muy fácil de usar.
+5. Adopta aleación de aluminio de alta calidad y material de acero inoxidable, no tóxico, resistente y duradero.
+6. La amplia apertura de la abrazadera permite montarla en casi cualquier mostrador o mesa.
+Especificaciones:
+– Condición 100% a estrenar
+– Tipo de artículo: PICADORA DE CARNE
+– Material: aleación de aluminio + acero inoxidable
+– Color: como se muestra en la imagen
+– Tamaño: aproximadamente 24x20cm/X pulgadas
+– Peso: aprox. 921g/32,5 oz
+– Aplicación: adecuado para carne de cerdo picada, carne de res, cordero, pollo, especias, pimienta y salchichas.
+Lista de paquetes:
+1 x Eje en espiral
+1 x Cuerpo de la máquina
+1 x Mango
+1 x Tuerca
+1 x Plato de carne
+1 x Cuchilla
+1 x Tornillo de mango
+1 x Manga del eje
+1 x Accesorio</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczO2ASc3xNoPDl8hvysdTx1YK3mi-Zv-v8u2APUouDYodSm7SdHEJv0bksW0obwekPo_gt9_tsh5Ui0U79qv93jC6w9GlH6ktm9fsaWApc7ORk5LdTtPB_7ObidAeoUk1Du8zDZbgo5vIfb-_pMdZNh7UA=w658-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNYyXsfoNC4mA5G42-c_iLOm3vno-yXQh1rK8kEfad1XqufW5HTNGdqA1uTxbaA4HPi8l74bSziaVq2JvA7XZ9FZnJzELFdIcUDN4LVnuskLzLjXx9M6wG2pp3iQ9eTpWB5c5Siq3ixV7RkmUzkyNXqbQ=w644-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMy1Q9grHFB6azn_lDL16C8virUnoK1NRERyQTQz65iHVUYW8_thvTAcWEqShKSiZTt95Eraw3PRp_Jdtg4ILhgZjNHgR-zvvd8y2DZgZchMGK5c2jqS5h69jaAN8qKivi8djrPYEoRVGbonsS1aw9ZFQ=w643-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczP3sPYzJs0TieJ8v1kSD50mYYweYKMwWszik8YzI1BNeufAAYAQb5uvtOVXkipxis_jaxTE7gg7_tx2Z4kz1AGQaKamPZEAK94s94TBrtKdzvb5Wzjxjb2D0aElUYzg4jL_IU8rslvDvfW723dtj5J4jg=w595-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczO8-mDmxS1h626MhA92jpb0S658-gNb0YOKyIoGEpQj8bLcuIzg3Rl-ff9Undw3ppqsxKonSXbenhX5f7vOCjOFWfXMOEgIAm4ADqg1YyWl4N0iwJnWfk00e4NjE5g24hVngGbp-norJl4PrZJKqB0QXQ=w633-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczO31gGEj5_zwP2WT9U31rDMxkaE13PuhjwapwzxvVelsbcenEtxpZmz6sMRUBPbC4A8FGdap_6nfyDrnvZEhSM-PuBDC0sri3XHRLlo8lE5KMvT49LqV9G5Ar2U6oziyBGTgQmg_isgZnMds4Nr0OO6XA=w637-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMJX-n-ppC9jgrsRgmF5yov5vXB8TubAeRzmVzoN3GFTWF1e4cdDElYRZT_jE6Xk7tPJ11xIKKCUF3PHCZExx0cNmTEieuIh5cKjCUkOhMwesKIFKTh5vgal7t9gi0_WisA3BO3nGZqbpGKZBubbirRgA=w464-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczORap2cghNw_A04efLOBD5y95nnpzqix2cxQiwAGG77Pmi0uMfe4-zg-9UcCiyOyCk9zRliDrLg-5OVNlQFhzo4R00A9rUFstktA2EBKkEY7MZpm8mSwxHGNWqO52Cqpdn1yhA4K_Dzl542vfCb57IJkA=w667-h633-s-no-gm?authuser=0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +543,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,10 +599,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -414,8 +620,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -718,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,13 +1275,13 @@
         <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>81</v>
@@ -1082,22 +1290,22 @@
         <v>65</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1105,28 +1313,28 @@
         <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F14" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1134,68 +1342,737 @@
         <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="345" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
agrege mas productos de la pagina
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\PROYECTO E-PLAZA NO TOCAR\E-Plaza.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F1CE5E-1899-48B1-A6B3-3C4545EA1264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DA9653-FEA1-4F2A-9C9D-30E529FB7C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
   <si>
     <t>image</t>
   </si>
@@ -70,15 +70,9 @@
     <t xml:space="preserve">señora 2 </t>
   </si>
   <si>
-    <t>señora 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">señora 3 </t>
   </si>
   <si>
-    <t xml:space="preserve">señora 4 </t>
-  </si>
-  <si>
     <t>señora 5</t>
   </si>
   <si>
@@ -238,16 +232,7 @@
     <t>17</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>13</t>
-  </si>
-  <si>
-    <t>20</t>
   </si>
   <si>
     <t>130.000</t>
@@ -367,126 +352,6 @@
 1 x Tornillo de mango
 1 x Manga del eje
 1 x Accesorio</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>60</t>
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/pw/AP1GczO2ASc3xNoPDl8hvysdTx1YK3mi-Zv-v8u2APUouDYodSm7SdHEJv0bksW0obwekPo_gt9_tsh5Ui0U79qv93jC6w9GlH6ktm9fsaWApc7ORk5LdTtPB_7ObidAeoUk1Du8zDZbgo5vIfb-_pMdZNh7UA=w658-h633-s-no-gm?authuser=0</t>
@@ -926,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -965,7 +830,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>11</v>
@@ -985,16 +850,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1003,7 +868,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1011,16 +876,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>15</v>
@@ -1029,7 +894,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1037,25 +902,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1">
         <v>23456</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1063,16 +928,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
@@ -1081,7 +946,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1089,16 +954,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
@@ -1107,7 +972,7 @@
         <v>23456</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1115,25 +980,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1">
         <v>5432</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1141,25 +1006,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1">
         <v>9876</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1167,16 +1032,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>15</v>
@@ -1185,7 +1050,7 @@
         <v>56223</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1193,25 +1058,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1219,860 +1084,260 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="345" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="D20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
agregue mas productos a la tienda V2
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\PROYECTO E-PLAZA NO TOCAR\E-Plaza.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DA9653-FEA1-4F2A-9C9D-30E529FB7C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFB1880-B62E-455D-A494-D6F06363B968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="130">
   <si>
     <t>image</t>
   </si>
@@ -376,6 +376,117 @@
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/pw/AP1GczORap2cghNw_A04efLOBD5y95nnpzqix2cxQiwAGG77Pmi0uMfe4-zg-9UcCiyOyCk9zRliDrLg-5OVNlQFhzo4R00A9rUFstktA2EBKkEY7MZpm8mSwxHGNWqO52Cqpdn1yhA4K_Dzl542vfCb57IJkA=w667-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Carpa Campin (3 personas)</t>
+  </si>
+  <si>
+    <t>Carpa Iglú Dome Para 3 Personas.
+Características de la Carpa Iglú Dome Para 3 Personas:
+Material de poliéster resistente a los rayos del sol y a desgarros. Peso inferior a 2 kilos, facilitando el transporte en caminatas.
+Varillas de fibra de vidrio y piso de polietileno, proporcionando soporte y comodidad. Incluye bolso para almacenamiento y transporte.
+Alto: 95 cm
+Fondo: 200 cm
+Frente: 120 cm
+Material: Poliéster
+Material piso: Polietileno
+Material varillas: Fibra de vidrio
+Resistencia al agua: 450 mm
+Composición: 1 Dormitorio
+Capacidad: 4 personas
+Uso: Ideal para paseos y camping.</t>
+  </si>
+  <si>
+    <t>90.000</t>
+  </si>
+  <si>
+    <t>Maquina de coser mediana</t>
+  </si>
+  <si>
+    <t>150.000</t>
+  </si>
+  <si>
+    <t>Voltaje: 110V
+Rebobinado automático.
+Trabaja con 12 puntadas diferentes.
+Tipos de puntada: 12 patrones de puntadas básicos.
+Tiene enhebrador manual.
+Accesorios incluidos: 1 pedal. 1 bolsa de hilo. 1 adaptador dc 6v.
+Ideal para proyectos de corte y confección.</t>
+  </si>
+  <si>
+    <t>Cinta Luz Led Con Control RBG</t>
+  </si>
+  <si>
+    <t>43.500</t>
+  </si>
+  <si>
+    <t>Cinta led RGB
+Voltaje de funcionamiento 5V DC.
+Cambia de colores con el control de mano.
+Longitud 5 metros.
+Adhesivo en el dorso para su instalación sobre cualquier tipo de superficie.
+Bajo consumo de energía, super brillante.
+Esta cinta led puede ser utilizada en TV, monitores de ordenador, consolas, equipos de sonido, cocinas, coche, fincas, decorados de habitación, etc.
+(OJO no es rítmica).</t>
+  </si>
+  <si>
+    <t>Maquina profesional de Peluquería VGR 665</t>
+  </si>
+  <si>
+    <t>97.000</t>
+  </si>
+  <si>
+    <t>Diseño de apariencia de moda, riguroso control de ingeniería, calidad garantizada, para satisfacer sus necesidades profesionales.
+-Cuerpo aerodinámico
+Diseño ergonómico, antideslizante, cómodo de sostener, compacto y portátil.
+Nueva actualización, transparente y texturizada, con personalidad.
+-Silencioso y potente
+Procesamiento de reducción de ruido, motor potente de 8W, recorte más suave y silencioso.
+-Hoja de acero inoxidable
+Afilado y resistente al desgaste, no se oxida ni calienta fácilmente, ángulo obtuso en forma de R, diseño de corte de 30 , sin pegarse el cabello, sin daños en la piel.
+-Pantalla digital LED
+Monitoreo inteligente, pantalla digital de la potencia restante, manténgase al tanto del Estado de la energía.
+-Indicador de lubricación
+Para obtener los mejores resultados, Coloque unas gotas de aceite en los dientes de las cuchillas.
+-Indicador de carga
+El indicador rectangular parpadea, indica que la potencia de la batería es demasiado baja y necesitas recargar.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPm0dbIwB6N1fkzH1GOYmB2Vul5L0C_WtjuYPUGoK1lyYIRnWr9N5AGGXd1OD6ZLjzU6ShnxtKtKC-hIjHLaB2_4dQqDioKGUpgpuvpvX6c0lb6q5FYBJyN50p9Zxd5h2xh86-BewzXhsXUZY904ruMng=w633-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMavoMtc3WjLiIMjJzpYPaBpGERxBJXtr9AzbulnQIDnH9QGgC-ne9RSP7X_nJM9tt0dUhlw_EPRVrVaBw5dGDZI-j1liNgOEfnt2pjkGnK2ppDuAmfnHxaOAawWWB3IRXAh1pXjinH4JFzTboix3mHAw=w710-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczOuTBTaOf_UKl7xmkVVmBGgBkhGOx-8zTCurHj4KVfO84CZrUr9zlCv1m5LCiPsk5oSCv3XQLHYrWMLQ8pyxJ35uhIoRJ-0gDs2DqsURpur8cQREnczPuFPmLspNH2fyeIyI4Qby6z5E4qbTlpsg8RBQw=w500-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczM2J_jvJwmXjcbDf04k4LnVV0JsMx0NOJ-6e07j_1v3OgOIbu2Gh3u8m6hXM5sFeldyPnHvP86oQqqt_29AL1frNv3pJ8h5ptZI5LsxQ_42UxGCMZBGHLJ8iNCBFMEEDLbRLrH2tZxpqF2C_7Y7c8Edpg=w424-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczO-3bzW3c8QT2SIsRPARJH_UZqz7q1FRHnnvuL956iyMPczbn-8pgYOsq1oxpwNj0P8QZVh-ID3LfzoFe3aO3IkzRbDrS-pZsTRR3Tvqcj92f5s4ox-DMKycR2SAe0qykH9KeD_cMtnMyUw8crLNH8bTA=w500-h478-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMbwBGr5UdIZphocvvyUsLRWOU_stL8c-IToMuKuWoWeTSFei-94O8cuxTdj50jCY1xE-iHNNIeoDB56DrVL6KI3KCCRuuh7PUMmI6MRq5kCn47GEPZ1QhZ-4H30ipdsCvYzntGm0ojDbM9YFNveN185Q=w626-h633-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNuSSgSUOaG-ylfAi-kKTBPKavs_z05lWhJCe7qhBZMHOmx3j8ma1I1TfZjymw2fHoxoDMd0yUTwH_EoUpAFLxSxNtJ3D1Vx9XWRP5fWzOB4ZbGk8zwFnHCpnzOx0EsqOj9lev2ZIZsi0o4p97ciLhgxg=w619-h633-s-no-gm?authuser=0</t>
   </si>
 </sst>
 </file>
@@ -791,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,8 +1447,199 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D20" s="1"/>
+    <row r="19" spans="1:11" ht="330" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
actualizacion V4 Productos : 43 //junior
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\PROYECTO E-PLAZA NO TOCAR\E-Plaza.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8F3C46-CEE9-4F80-A650-72E619DC6B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C0887E-B958-4ADA-B5B1-441A1E3606B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="277">
   <si>
     <t>image</t>
   </si>
@@ -633,6 +633,584 @@
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/pw/AP1GczNdyqVrV3ZLafUKC5b4c-SCO2eIejocSPdP1JTvXjHi2leE2oS84AHmiudmdbeC5vrs4FNygBTlN9G2MSxjSCaW1QRydGkIq3ct3AVOZ-hZxVi9xCabcPy4YH1HUnhCzG0prIk0aMTkMfbU0rfSE9m6YA=w500-h366-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczP2M-v19tMTe3_kE2kUYF5C5_Up0BwFb6tmDSrIxIJmTZl7yQ5R_OOJNma73CUUtAsZ9Jk45Pl18DeuaW3fAWW39P1-ACWb6CXU7CSgRmfhlQNl1LO37BMaf-BA8Sjk84OCShi9cTNsJDeJk1khuqV4dg=w340-h340-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Tambo police defensa personal</t>
+  </si>
+  <si>
+    <t>40.000</t>
+  </si>
+  <si>
+    <t>Tamaño cerrado: 20 cm
+Tamaño Abierto: 51 cm (completo). La vara se expande 29 cm
+Peso aproximado: 480 gr
+Secciones de pliegue: 2
+Materiales:
+Vara: acero inoxidable.
+Empuñadura: Goma en polímero ergonómico.
+IMPORTANTE: es completamente normal que el tambo se atasque una vez se abra ya que esta es su funcionalidad para que no se cierre mientras se usa. El tambo no se cierra a presión sino mediante un golpe seco contra el suelo o superficie solida (ver vídeo que se encuentra al final de las fotografías en esta publicación).
+El tambo cuenta en uno de sus extremos con un tornillo para asegurar el bastón. De esta manera se impiden aperturas accidentales. En el otro extremo está la vara, se abre con una sacudida (golpe seco) y se cierra con un golpe contra el suelo (ver vídeo que se encuentra al final de las fotografías en esta publicación) .
+Es marca Police de Shen Suo Gun. Todos los tambos de los que disponemos son en color plateado, no hay otros colores disponibles ni tamaños.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczP8dabF48jo0JTMy1joQYZWS1iuxWEHBFIsUI9L-ORFKaLrOWxE8q96v2e-Xs_l7V8sfjQm0e00OFUZaMfE-SjcHOSB0RUVTDoTDms6824dCe15XA0fE55UCMgVpB1Hc-R2Qs788ynkdvxMP-RZXxk87A=w500-h432-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMhaKLnNNtCh3PW9gnUiX5E6Pv2hIieESjdcNrHYlH-5LNSAexrnPhkXsoCbEB_zxVpo7TATckqVImnRnl2VgeBZcA4kA9YYeqNXoFwHU0E6fs1Klh1-3n7MMcPVbpT8bvYFMnhC4BvcSJ0TWdCX68ocQ=w500-h448-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNZ7DmyDxlYZnNd0fnD33CHthsuwyMqN8heivE5wiRNAe7YKNEUCw8yatznGAq2dZkz2357ACLdw11GIxrV0ulALYRY9PLknAyS9xaMhqR4s7svdTvYaZFbsRVOfY0dsHdcIWfGvsQeigigZUOTwzjs3A=w469-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Camara Ip Tipo Bombillo 360º Robotica Wifi Vision Nocturna</t>
+  </si>
+  <si>
+    <t>72.000</t>
+  </si>
+  <si>
+    <t>Mantenga un ojo en su casa en cualquier lugar y en cualquier momento a través de su teléfono inteligente, puede girar para ver en cualquier lugar, 1080p y clara Full HD resolución proporciona una alta calidad de vídeo en la palma de su mano.
+La detección de movimiento: Esta cámara inalámbrica tiene una función de detección de movimiento,activada por medio de la app. Puede configurar la advertencia de voz de la cámara y también puede hablar a través de la cámara para que puedan escucharte.
+Vista a distancia por teléfono, sin importar dónde se encuentre, puede ver la pantalla de supervisión en la aplicación en cualquier momento y en cualquier lugar, y se puede hablar entre sí a través de él.
+Uso de camara para interiores.
+Modos de visión diurna y nocturna: Es una imagen colorida durante el día. La imagen es en blanco y negro en la noche.
+***NOTA IMPORTANTE: Por proceso de actualización en aplicación es posible que en 1ra configuración la imagen de negro y se quede cargando ,esto es normal, por favor si sucede esto resetear al cámara ,re agregar la cámara en la app y volver a configurar, ante cualquier inquietud comunicarse con nosotros***
+Tipo: cámara IP
+Alta Definición: 1080P (full-hd)
+Lente (mm) : 3,6mm
+Color: blanco
+Megapíxeles: 2MP
+Cámara de uso en interiores, no apta para exteriores</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczOjXUeTqqAKqZuSYlU_0wh2uAeljClDm7xYyndmdyrKgsEYyS2UeaGW_h7qrru5uE1NjDD97b3nDmC9-eYUXFXSWeJ08gMU-m5iL-AzYrHnKDDsvb3_4Px9nZdaoiEYU2v6cKzDAsvB9X2cz3i0nhKlZg=w500-h392-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPXExvIyVq2-M_1BEfHWPjxnFTI42HItYxj72PzyDOLA-8vE19hWVH-Zp72qI3JJrx8AGbzO47nPIIbcRPfEl1nqUo9Mp4PasAfCLCSzefR9wFRbM5T6SSJW7g1jiuJxo8JeYa90sDSbJzheswQQgslmA=w500-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPMycV41RyGr2LWzZhA6MGIGxAd5FdusGyCGRD137hMIDrTBudsDt8IFbPPtu7bIzapm_QiSXY67XlIi89cW5Ok4b6a8aqBQUuCxBGAJfTBtLVUU9YtKOJnXw1c3laC_ms22j1ADsHTMp05o3BR7GW7SA=w500-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Teclado Gamer Numerico</t>
+  </si>
+  <si>
+    <t>Teclado Gamer de la marca jeoang</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczO84y__W0ru0xe4Em4YNyCPfJPFAQAbHm8FPBihU0mrR5jMiLnWwq3q5veAlCD3q_45bSJG5xnwEFd7gPlhzjnMc2JJVUal2Y2S2H54rwYM6nu2XTsw3dKg2B8RUnmOVnahXUgDQceEMOSSJQ5ZODoymw=w463-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Mouse vertical inalámbrico recargable Weibo WB-881 negro</t>
+  </si>
+  <si>
+    <t>57.000</t>
+  </si>
+  <si>
+    <t>Lo que tienes que saber de este producto
+Contiene usb inalámbrico.
+Puede conectarse a cualquier dispositivo a través de Bluetooth.
+Incluye batería recargable.
+Posee rueda de desplazamiento.
+Con sensor óptico.
+Resolución de 2400dpi.
+Creado para llevar a todas partes.
+Control inteligente y navegación fácil.
+Adaptado a tus movimientos
+El diseño innovador de este mouse es ideal para actividades donde pasas mucho tiempo en la misma posición. Con este dispositivo podrás descansar tu brazo sobre el escritorio y disminuir incomodidades de una mala postura.
+La funcionalidad al alcance de tu mano
+El sistema de detección de movimiento óptico te permitirá mover el cursor de una manera más precisa y sensible que en los sistemas tradicionales.
+Plug And Play
+Solo debes colocar el receptor en un puerto USB de la computadora y ya puedes empezar a usarlo. No hace falta emparejar el mouse ni descargar software para utilizarlo.
+Conexión en cuestión de segundos
+Gracias a su tecnología Bluetooth tendrás la libertad para crear cuando quieras, donde quieras, en la computadora que elijas, con toda comodidad.
+Mayor duración de la batería
+Con batería recargable incorporada que puedes cargar fácilmente con el cable USB incluido sin necesidad de reemplazarla. Para prolongar la duración, usa el conmutador de encendido para apagar el mouse cuando no lo estés usando.
+Apto para fácil traslado
+Navega rápidamente por documentos y páginas web gracias su diseño ultra delgado, ergonómico, liviano y conveniente para llevar a donde quieras o viajar.</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNz-moNkDVWmKabpuaFrDGsme3E8z1OI7-TjoFE0lg5TT7P4EnMFDP9XY7nJMROaiRFh7yPnYrIxQdL-d9Z18x-YbkWImD1q2PIyLEpKeRLD7D7Ks_oTjVKZYQX1VF1Tt8qINxXuVZ6l70L3EGpO8139A=w600-h600-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Aro De Luz 26 CM Con Tripod 2 Mts</t>
+  </si>
+  <si>
+    <t>Aro luz led 3 tonalidades luz, 10 intensidades de luz.
+Aro 26 cm diámetro.
+2 MT trípode.
+Control alambrico
+Soporte celular.
+Verifica nuestras calificaciones.</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczOLYiw9sAMDvLUuykcXMJXnPcahs3KTc3QFyY4H1jSvomcr-4QqcoFGkihsEUF_T_taxAqe8Wu32lh6QZuOyO3AUAnX0XH5fc5fd4CrKABC7olFQOIsO7F-WXLdxcmT3PVYFAlm82XRMaMs2YbZQkQE4w=w500-h283-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Reloj Smartwath x7</t>
+  </si>
+  <si>
+    <t>El Smartwatch X7 cuenta con una pantalla táctil Full Screen de 1.54", ofreciendo una experiencia visual intuitiva. Es resistente al agua, soportando solo salpicaduras, ideal para actividades cotidianas. Compatible con sistemas operativos iOS y Android, se conecta a través de Bluetooth para una sincronización eficiente. Su memoria interna es de 32 MB y está equipado con una batería de 180 mAh, proporcionando una duración adecuada para su uso diario.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczOBFyoOjpH3iuGeJoM_qe2Fvt1-DTAJP031ck3uW19PNkrNRyBOge9EPoDDCOavYyZ4ePk0ZMeHAi1h9Z07a4EsicyQwQLAUxb2oMgXQsPm476kvEpBnBO1HAgSkfqeXc5Sbf00d5iKVAWGZhbm8pIfuA=w500-h499-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNPZa9-xBRIVT99PhE5VzC7D9FNHhZKcMtnQRnsUjVA05pam1pNnS83JsXkxxJ8B7k2gUtrt0_rX3zUGgnPrXLHYdrhPiQgQH-pssR8SmbkXvfg8OZPqUfT6h3Zu5q89HvqnQMuoChc020bk4k_4bdhdw=w400-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczO7FtzoHUNfc4nesK1c6joQzV_Eh7trCRmjoRFjYTZNTaBTnnE3cI8HY5bWTOsSOiHyuzPb3z4_0Gg7ajouA4MZlJzEI0YtZjcnl1UpDYztSHG-tu8bnm2t1SvIx0xQqL_C0BRBv4dyJDR6zUNyC9IQTw=w500-h359-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Elévate 5 CM</t>
+  </si>
+  <si>
+    <t>30.000</t>
+  </si>
+  <si>
+    <t>Este cojín de tacones aumenta hasta 5 centímetros de estatura de manera rápida y discreta. Fabricado con plástico de silicona flexible, ofrece comodidad y resultados instantáneos. El juego incluye 5 pares de plantillas, con 5 niveles diferentes de altura para cada pie, adaptándose a las necesidades individuales. Es fácil de usar, discreto y adecuado para hombres y mujeres, encajando perfectamente en cualquier tipo de zapato. Las dimensiones del producto son 16 x 16 x 3 mm, y su color es claro, asegurando que no se note fácilmente.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPOn05TAMGglpSfMtzv1eWFTX44RKtgl0pfUWOyvpkeAO4imoaOsSJ4dCmWvtkWwNrLEcHHALAOcr5Mn71edQ14rg70KmXIMTTdf42X2dj6IObfgGPuBC5MFuV_hDBp4WW2lisWqn1JI63ItZDuG9Gs_A=w500-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczP39QJwtGZAyJoyizYPXlJeyHuUu1kuz9Eifbqy8Q3M6uojIVfbheTrpv5LlMtF0hiZuGiYmd7HZLMVUxi_wpROUtDg2ki8wGo4TGmXM2qU3TSZP-HRH0B3vD4wk1_zZqlX6aa7mFGER1yUgOMvpc0Agg=w500-h463-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPFvDcgyySOYIMrqtA7cIaQ0sm27BW53kwlYLWcZSs7JrJTLJ-gMEPCyiI4HQYJKh7vUEm0DIgEqRG1xs0VHA7hFAHBWhhoIOMUfiMqJ-1RHhaLmJrxy9ppeNxGGqte7U6bKq8uN--sXvTV6LSw72YpVw=w479-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPzVqqBRrl2qn2eGXPtw0s2DnhF9W44-ypJGRp-wslAO2mPGIIprGW3PJEXlSXvgH9DaQEPtiHCGAnha9sGZe3SS12ZzUMhMFMnfc2bgSPkNBrRsUualRWkAyten2isrqoa_vpPJRgc2AwO7rcfbiGQYQ=w584-h616-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Guantes Para Dedos, Fundas Gamer Antisudor Pubg Free Fire</t>
+  </si>
+  <si>
+    <t>18.000</t>
+  </si>
+  <si>
+    <t>Uso del producto:
+1. Retira las fundas del empaque y úsalos en tus dedos para jugar en tu dispositivo móvil.
+Cuidado:
+Lavar a mano con agua y poco jabón
+No lavar en lavadora (Daña el producto)
+No restregar
+Revisar el estado de la pantalla del celular (sin grietas), para asegurar la duración del producto.
+Características:
+Material: Fibra de Nylon.
+Se desliza bien en la pantalla.
+Resistente al sudor.
+Protege tu pantalla táctil.
+Elástico.
+Se adapta a tus dedos.
+Compatible con todos los juegos.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMHZYsXK5k_cFjUHdQEOdESHtZWm-DoqmNMfe6yqS07fKaWreRifAOi5Yy-wNVsnoneYTq0r4AP_ACt3vc9c237lRm8ugwOY7lPrxEeayz3WTo8NTRW85WSbRSKJl2JBFK80pEHWr_5owkodhxktoEXdg=w605-h565-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPA_vUxUsSff3RUZRea-7V3cc0fOEa3xV1fRDTk1Ir5Bcly4he6qAPD7Bs3RMBgQ3Ul_Yt24mqSlIO5tsooGwKi9hiKTuhi4isZIH1GfqcFAhOsooXiz6gAT1_KCoYZ1pMSDykeB_4FviLSWX_Mmp0wrw=w482-h482-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Tabla Picatodo 3 in 1</t>
+  </si>
+  <si>
+    <t>43.000</t>
+  </si>
+  <si>
+    <t>Tabla de picar multifuncional
+– Práctica tabla de picar con tapon para almacenar agua,
+– niveles de profundidad
+– patas antideslizantes.
+-Manijas antideslizante
+-Diferentes niveles de llenado</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNaQux2MQyb9yj40mBQACC6dV1GVUl3OYQGxEGjtYMflcuWj7bvbTbFu05AC6EUZs1fNPEaUtT1cW1vfWDPVAVniEGgp2NFZDbE05JyuXR7mypM8S-CavZMwbUqs_naXHMZ39-ZvydPISb_WgrVcrzMVQ=w720-h736-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczM_jnnqycv1-E0po1-mIns9VupwArhweKnWqGInnVP-Cp_N5bWUKNs-MBVCqlezQrihvX11n6zbG_C5J3AAl2dlsLyI8hFA2tQS08ObjsJr9UvvpQ0V5UILa9lZ_xgm1LXfDpPMeyFpJJHHa_pWHKHgJA=w720-h716-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNaB1OxURteMy0rFd7g5-BlO8USFuFf9yNp0ie_mI0zMCWhYnj978Qlwdtd9EElLtlsQVvi6wS6v2KI7TzpFOouRTGrsIIIVhZ-VVx166lB9QQ5fReSQHAW8KOP6lXLu_xEn4qHTmZaRXbS1DoWQOfa1A=w813-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Llaves Multiuso Universal Snap And Grip</t>
+  </si>
+  <si>
+    <t>32.000</t>
+  </si>
+  <si>
+    <t>LLAVES MULTIUSOS UNIVERSALES
+El juego Incluye 2 llaves maestras que se adaptan a todo tipo de tornillos, tuercas, tubos y hasta tapas.
+Usan presión en 3 puntos consiguiendo una sujeción firme y estable. Se adapta a la medida y forma de tornillos y tuercas, tanto si son circulares, hexagonales, cuadrados, sean del sistema que sean, incluso hasta tuberías.</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Gancho Porta Celular Flexible</t>
+  </si>
+  <si>
+    <t>25.000</t>
+  </si>
+  <si>
+    <t>Adaptador en forma de gancho, para  su celular, manos libres, cuenta con clip adaptador para escritorio, repisa etc. Soporte flexible que posee un clip o gancho que se adapta a cualquier superficie, es universal para cualquier celular, se adapta a cualquier posición. Facilita la vida diaria permitiendo realizar otras tareas mientras se escucha música, ves vídeos o películas.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczOrDDIybJm1OT37-0P1IhjmYnr4BO69zl7tspmaqitkhtrB2RAZDIEzUBEqm5qSfXiE7Sm1RTBlbFLa8fKPICrONSC1mH3vzIUnlPbQp3Az3JOrOsLNk_l-pxR_tG-YaoiRjq3EPdFswBHruio_Snk8NQ=w340-h340-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Maquina Peluquera Profesional Gm-1030 Progemei</t>
+  </si>
+  <si>
+    <t>86.000</t>
+  </si>
+  <si>
+    <t>Cortadora de cabello profesional excelente para su uso personal y profesional, cuenta con un motor de tecnologia innovadora que evita el calentamiento de la maquina en un 40% y trabaja a una mayor velocidad de corte para lograr un excelente acabado y mas a ras, tambien tiene cuchilla de acero inoxidable que son ajustables para variar el largo del corte.
+Contenido
+– Motor de Gran Potencia
+– Cuchilla Ajustable
+– Kit de Aseo y lubricación
+– 4 Guías de corte
+– Peine</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMh2MEVSBFF9Ypp1xQrVZU_agrkg91dnAasBNWp4rggc9sEX80O8LPAyBSAjwheLhxmc4cTEcOVtbr9YkSaqD5lt1e0OEVLcENxlGa3-Y-4Z2bOPb1d5K1sscldC7zAlXf_9x5C01JKCHViPc16h94W6g=w600-h600-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPq0I0WKsxBWVVaDdg_c_2xUpaQSIpTsFyFeaR0rRjgwQ6FnX6tEC0-axtBDiL1I3KCMmmF8dFpwMGrcYO-vWteIbN73QGRoME9HgeYEq9nFnbL5UGHKdUFC1RIuIRt7lhRzTVcx6jhJVjzgKpFxb_kWg=w450-h450-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Afilador Cuchillo Con Mango Ergonómico En Acero Inoxidable</t>
+  </si>
+  <si>
+    <t>Afilador de cuchillo con mango ergonómico antideslizante en Acero Inoxidable
+Este afilador de cuchillos profesional de tres etapas permite afilar de manera rápida ágil y segura cualquier tipo de cuchillo.
+Es de tres etapas:
+1 Tungsteno: es el primer paso, da un filo brusco y fuerte en pocas pasadas (recomendado dos pasadas)
+2. Cerámica: afina el afilado en sus ruedas de cerámica con el mismo procedimiento
+3. cilindros de cerámica forma diamante: suaviza el filo y la punta
+No necesita ser muy profesional. Solo tiene que poner el cuchillo en el afilador y pasarlo varias veces, el resultado sera un afilado agudo, como si fuera nuevo.
+Notará además que la vida útil de sus cuchillos será mas larga y el filo mas duradero.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNuvi6ctdTGO_X0ysIMgF5oQSqSS9VSL5yvS9K3I17f_mJsilOaxEgrvSxQGSML85IpMNVdhntKyOrXb001mxhQ5SH8SHLEwWl9xhvQCQ7v50zCX0iEmGPOrr8-c99uDKmu6p5Ad46PNsZEPghP4S6JWg=w791-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczObp-cvatxaA2Cw-hwW3DPBWkCULeR3ohFbBHMBI0JOgIa5sx2AF2xoOtz12umzd4t5ingAdirtn0CV7Q5VsM2JHGdfqTi0EI4SW7TpDxxawXjeaMLtGFFzZj5njFzhm5i3Ndv0dCsvR8HF6V2TwswSug=w788-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Repetidor Amplificador Señal Wifi Router 300mbps Inálambrico</t>
+  </si>
+  <si>
+    <t>71.500</t>
+  </si>
+  <si>
+    <t>El repetidor WIFI, también llamado Range Extender se utiliza para ampliar el alcance de una red WIFI. Un repetidor WIFI funciona al recibir la señal WIFI de un enrutador y luego lo amplifica y retransmite a nivel local.
+Con un repetidor WIFI, las computadoras e impresoras ubicadas fuera del rango original de puntos de acceso pueden acceder a la red WIFI extendida. El repetidor WIFI duplica de manera efectiva el área de cobertura de su red WIFI existente, extiende su red al otro extremo de su hogar u oficina, solo necesita ubicar la a mitad de camino entre las computadoras y el enrutador.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczM_jEsW9AHgdZpJajcgr6nYcw5kfOylsDjj4C2xo9Sl3pK1EKbzCgYGPzoBjW2MCLkLPGy-nxKH3Js7tbC8UTYwRdnghF7DBAkmWQqLfD_sNe6b3bCfTdWPNAFjjwG7TUv1ib2u0R1FNNTORsafbudlgQ=w500-h500-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMbozyCKQi-fBNAy2fdBGZLD43GfBVvaF4vly0xUc3eSBzWXaDLgu7CpgWSuZK06lelgh2QxmiUOy1-dzAZhCr8CSgz9MNtf_fPpVZLsAGbx49j8FEAgbyVTMjmgiOLLPKmLzgLG5dOfQfgbrK5_8zfrg=w791-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMOg3Z8KTaZPQeXRX7HkTzD51_trjPhvOza7yOZ9MAL3vDh6oYGEFS1g_7Y7iAwp7ERQBXFQSlciH2nRx2XQna67-ppaFkjkqd9d0F1muA7l73jOj2pRE6hdwNeNFWMk2qHJGoaz2L6V0fuTJbp477uxg=w640-h640-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Lampara luna y Estrellas</t>
+  </si>
+  <si>
+    <t>55.500</t>
+  </si>
+  <si>
+    <t>Lampara proyectora de Luna y Estrellas
+Ideal para que sus niños concilien el sueño con mas facilidad
+Linda, entretenida, novedosa.
+Disponible Morada y Rosada
+Mas de 10 colores y combinaciones diferentes
+Funciona con 4 pilas AAA o se puede enchufar a la corriente DE PARED NORMAL (mediante adaptador tipo celular no incluído)
+********NO OLVIDE RETIRAR LAS 2 PROTECCIONES SUPERIORES DE LA LAMPARA, PARA PODER USARLA******** para que le pueda dar proyección a la pared si no le quita la tapa no le da proyección a la pares si no que sera una lampara normal que no dará tanta luz para la proyección a la pared hay que quitarle la tapa</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMF2jtI1b2cNKXwPZFgHbWBJ78utU6oQT0mWWDRfzAKeD7eSW_dNUSPj1SQvxiKr79szs3agMbYUB1rSrpAp-RfWR0WbSEYIQB73PSXRXlkTCpcWexe00y_7WQEQim9la-VpFSq0vNk44VSoMwnJj1StQ=w320-h317-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMd-Z9zHNj-_lPPiyjzStSl4A3M217M-C2nT1gc1Pw3RFEyioaGKQgshEb8_kKpg6Dps2yybUTn0NoXHFX06swdKSXpDzCHPJI3jMDjC0VvjC3Wq-YT2RqzZG9dm_L0P9xsrirpUA6sTLvvr9ahKV5O_g=w791-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Bombillo Parlante Luz Led Multicolor Bluetooth Control</t>
+  </si>
+  <si>
+    <t>38.900</t>
+  </si>
+  <si>
+    <t>Bombillo Luz Led Multicolor Bluetooth Parlante con Control Usb
+Bombillo Led parlante Bluetooth, con este dispositivo podrás escuchar música vía bluetooth, apagar o encender la luz con el control remoto y cambiar entre los diversos colores de luz.
+Características:
+– Puede ser controlado vía bluetooth
+– Apariencia de la lámpara LED
+– Conexión inalámbrica bluetooth
+– Base de la lámpara E27, tipo tornillo
+– Volumen ajustable de luz y música.
+– Luz brillante, comparable a una bombilla halógena de 50 vatios.
+Especificación:
+– Color de la cáscara: blanco
+– Interfaz: E27
+– Voltaje de trabajo: AC100V ~ 240V / 50-60Hz
+– Potencia: 12W
+– Potencia LED: 6W
+– Potencia del altavoz: 3W
+– Respuesta de frecuencia: 135Hz a 15KHz
+– Versión inalámbrica: 3.0
+– Configuración de soporte: A2DP
+– Gama de radio: 10m (33ft)
+– El color de la luz: RGB 16 color con el mando a distancia.
+– Amplificador: Clase D
+– Entrada de señal: bluetooth. (2. Transmisión Bluetooth 4G)
+– Distancia de transmisión de Bluetooth: 5-10 metros
+– Contraseña de conexión Bluetooth: no
+– Temperatura de trabajo: -40 ~ 80 grados
+– Tamaño del producto (L x W x H): 9.4 x 9.4 x 13 cm
+El paquete incluye:
+– 1 x lámpara LED (con altavoz Bluetooth)
+– 1 x control remoto (incluye batería CR2032)</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPer0Wcv6LiiYOmnUusZjCrrHDMrx-9-EzF7C4KA2VK8JAR4Qroi3Al9l0IybtaJU3YLqdNhhn7OkrFROxoCc-nwweQVOYETfnHSdi8dRAxVTBqVfhMyKzpWnYPENZPmqtoU7FQh-XZKtNjAp8oCkLZVQ=w600-h600-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPzi--RKkxJoRgtFqEK4TdsxXl66u4Ph6UZdqTxGMA_f-6DlLNE4vOf7QmjJZ1d0HxkplDxLnyMy3mEHAjZW5RJNDbxwMTyerNjsbDOfPbvBWETlC6hGP9S4fg--rktbR-cDfe1rrKJeltpgKhISBQfAg=w791-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Mini Tripode Araña Pulpo Flexible Para Celular Camara</t>
+  </si>
+  <si>
+    <t>Mini Tripode Araña Pulpo Flexible Para Celular Camara
+C1015
+DESCRIPCION:
+Mini trípode flexible
+100% nuevo, a estrenar.
+De alta calidad.
+Completa flexibilidad, hecho de plástico duro
+Ergonómico
+El peso máximo puede soportar: 0.5kg
+Dimensiones: 18,5 x 4,2 x 3,6 cm
+Color: Negro
+Para cámaras DSLR y teléfonos
+Ideal para celulares o cámaras (el soporte para celular no está incluido)
+CONTENIDO DEL PAQUETE:
+1 * Mini Tripode Araña Pulpo Flexible</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Bolsa Estuche Forro Impermeable Celular Camaras</t>
+  </si>
+  <si>
+    <t>22.000</t>
+  </si>
+  <si>
+    <t>BOLSA ESTUCHE FORRO IMPERMEABLE CELULAR CÁMARAS
+==============================
+MUNDONOVEDAD
+PRODUCTOS INNOVADORES
+==============================
+Para Celulares, CÁMARAS, documentos, llaves
+para sacar fotos)
+medidas: 18x10cm. cerrada (abierta 25×10)
+triple cierre ziploc + velcro
+Elaborado con materiales de alta duración, te permite manipular la pantal
+Contenido:
+1-Forro Protector</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Tripode En Aluminio Para Camara y Celular</t>
+  </si>
+  <si>
+    <t>TRIPODE EN ALUMINIO PARA CAMARA FOTOGRAFICA – ALTURA MAXIMA 102CM – ALTURA MINIMA 35CM
+INCLUYE ESTUCHE (BOLSA) PARA SER LLEVADO Y CARGADO
+Hecho de aluminio ultra ligero de excelente calidad para una experiencia de operación más cómoda y fácil de llevar. Antideslizante, ligero y duradero. Cuenta con dos perillas de control independientes para ajustar con precisión el ángulo de la cabeza del trípode. Incluye Nivel liquido de Burbuja para nivelar sus fotografias de manera perfecta. Es ajustable en 3 alturas (35Cm, 51Cm, 102Cm) para mayor comodidad de sus transporte y utilizacion.
+CARACTERISTICAS PRINCIPALES
+– Material: Aluminio Liviano de Excelente Calidad y Plastico
+– Liviano y Portatil
+– Ajustable en 3 Alturas: 35Cm, 51 Cm, 102Cm
+– Altura Maxima: 102 Cm – 1.02M
+– Capacidad Maxima de Carga: 2 Kilogramos
+– Las patas robustas de 3 secciones están hechas de aluminio y vienen con cerraduras rápidas.
+– Incluye Nivel liquido de Burbuja
+– Ideal para tomar fotografías de viajes o deportes
+– Peso: 380 Gramos
+POR SU COMPRA RECIBIRÁ:
+– Tripode 3110 de Altura Maxima 102Cm
+– Estuche en tela impermeable
+– Caja</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNsJM_aNOKvMcPLNsEgMQ2_yDzLsgGom2mYBl5c6xMs8OEvvxtSnHQTEnrtY4tQDLQFysSpLHSOGovTGg1RbChGae3SSFP5h3GXeKYfAGF2N-TLruveDuZLTJHpN18Dt9RkTLATx-C4Hc57I5cre9Plvw=w791-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Bombillo Lampara Fútbol 40W</t>
+  </si>
+  <si>
+    <t>Características:
+1.Apariencia como UFO Football le da experiencia visual, unidad de corriente constante, no hay luz estroboscópica, inofensivo a los ojos humanos y el cuerpo.
+2.Bajo consumo de energía y super luminiscencia central, protección de sobrecarga, protección contra cortocircuitos, protección contra bajo voltaje
+3.La lámpara se puede ajustar.Fácil de instalar.
+4.En comparación con la iluminación existente, el coste de mantenimiento es menor.
+5.Super brillo y ángulo de haz se puede ajustar: Lámpara de fútbol puede soportar 6000 lúmenes, por lo que es adecuado para grandes zonas de interior, tales como escuelas, hospitales, almacenes, líneas de producción de fábrica, etc.La lámpara tiene un muy amplio ángulo de haz.Ajustable
+6.Instalación rápida y sencilla: sin necesidad de herramientas, fijar la bombilla en el soporte de la lámpara de E27 sin necesidad de instalar las lámparas más grandes, tales como lámparas LED; se conectan directamente al soporte de la lámpara de E27.
+Consumo Energético 40W</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczMm6BXM1H4bEbQ7jSSvfAuXTva9nEbx1LiNPdnDAi-EY_hshXFxEcFVymwDbdR4pT2bx36KDtCuQHN2gBu0dxKe9_CzqLmK8cBkqUGfaC231-71yFJh5nEPh60vDu58GXYCRocC6Hs6i8kFsQrEjslpMg=w600-h600-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPNSFHF_4_4eXe1P0YDTV3pXYVyTTVmUZttLJx5mpHjdM06QODaOK7WHahBCFM2cdaKquNZLyzIf1lxIClfq31A7C2ZItUSnPlYEykhB9AH-JyUdWxG35lM47P3h4aU7VzjCmatfGyoaXDw0TusDJmb_w=w607-h543-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Gramera Cocina Digital Capacidad Hasta 10kg</t>
+  </si>
+  <si>
+    <t>35.000</t>
+  </si>
+  <si>
+    <t>MAXIMO 5 UNIDADES POR COMPRA
+CARACTERÍSTICAS:
+FUNCIÓN «TARA»
+PANTALLA DE CRISTAL LIQUIDO DE 15.24MM (0.6″)
+IDEAL PARA LA COCINA
+CAPACIDAD DE 10KG
+FRACCIONAMIENTO DE 1G
+PANTALLA LCD DE 1.6″
+RESTABLECIMIENTO A CERO AUTOMÁTICO
+EQUIPADO CON SENSOR «CALIBRADOR DE TENSIÓN» DE ALTA PRECISIÓN
+APAGADO AUTOMÁTICO
+INDICADOR DE SOBREPESO «EEEE»
+DOS UNIDADES DE MEDIDAS (G/OZ)
+UTILIZA DOS PILAS AA (NO LAS INCLUYE)
+MATERIAL:PLÁSTICO
+CON ESTA BASCULA DIGITAL PODRÁ PESAR TODOS SUS INGREDIENTES DE MANERA RÁPIDA Y PRECISA, LO CUAL NECESITARÁ SI QUIERE ACERTAR EN SUS RECETAS. ESTA EQUIPADA CON UNA GRAN PANTALLA LCD Y SIRVE PARA UN PESO MÁXIMO DE 10KG, APARECIENDO UN MENSAJE DE ERROR SI SE EXCEDE.
+CON LA FUNCIÓN DE PESO TARE PODRÁ DEDUCIR EL PESO DEL RECIPIENTE UTILIZADO O AÑADIR MAS INGREDIENTES PONIENDO PARA CADA UNO EL CONTADOR EN CERO. PODRÁ GUARDARLA CON TOTAL FACILIDAD DESPUÉS DE SU USO GRACIAS A SU REDUCIDO TAMAÑO. UN EXCELENTE AYUDANTE EN LA COCINA.</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczOgex5SuNLpHrIkZfF92MsFhIF73EPGxXwJdx6sfyJjry_p70SDkEnpGqY0EGnQswexs6XeA4EGzLKxrTN_ZCN8jw8qnrI7ZoJcDZxrtxNwAvZxY-YA_s6C2Jvvj8WqFnEkhTdpimjdoKeeP84gR4c0zw=w600-h470-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczOBcqvc9HHKeU9smkCRPduTuVkhuDR6zovGWNBx4N392TMneM_62GprDw3axjun6PnIi5YYVKR0f_RRyvL8oQfH8i3BjazVpDf9lktJLNE8z6zngtf92pMWWtCk4cDJtr6hXCoAiUYR8UoYRzER0jYsTw=w593-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>Flawlbss Recargable Portátil Removedor Vello Facial</t>
+  </si>
+  <si>
+    <t>Flawlbss Recargable Portátil Removedor Vello Facial
+– Llegó la Moderna y practica depiladora de bello facial recargable.
+– Luz incluida para ver hasta los vellos más pequeños.
+– Remueve vello facial apta para todo tipo de piel sin dejar enrojecimiento.
+– Remueve el vello instantáneamente sin dolor.
+Contiene:
+– Máquina depiladora
+– Manual de instrucciones
+– Cepillo limpiador
+– Cable usb</t>
+  </si>
+  <si>
+    <t>39.000</t>
   </si>
 </sst>
 </file>
@@ -1048,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,8 +1696,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>117</v>
@@ -1147,8 +1725,8 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>118</v>
@@ -1176,8 +1754,8 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>119</v>
@@ -1208,8 +1786,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>121</v>
@@ -1240,8 +1818,8 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>123</v>
@@ -1278,8 +1856,8 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>127</v>
@@ -1313,8 +1891,8 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
+      <c r="A8" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>130</v>
@@ -1351,8 +1929,8 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
+      <c r="A9" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>134</v>
@@ -1386,8 +1964,8 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
+      <c r="A10" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>137</v>
@@ -1430,8 +2008,8 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
+      <c r="A11" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>143</v>
@@ -1630,7 +2208,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1662,7 +2240,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -1697,7 +2275,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -1726,7 +2304,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1755,7 +2333,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -1790,7 +2368,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -1822,76 +2400,711 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="1"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>273</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="K9" r:id="rId1" xr:uid="{90117452-467A-485C-B610-C6F4271DA73A}"/>
-  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="10" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <pageSetup scale="10" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
solucion de problema de imagenes V5 // junior
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\PROYECTO E-PLAZA NO TOCAR\E-Plaza.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C0887E-B958-4ADA-B5B1-441A1E3606B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A2F1BF-3240-4929-BA4C-EB6917EC638A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="282">
   <si>
     <t>image</t>
   </si>
@@ -1211,6 +1211,21 @@
   </si>
   <si>
     <t>39.000</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPJHa75jloBTDJfai3A8k1UlRGmPeBUdm6HlhPD7fw-F-bkLTXRS9Ryj0zzOCcXhWyvz2muQaHRINOHM5TYyWtgla5NSrzpEzX9zzNEuaAwJ4rYpHiiujs2ILVoK1BmHcBGuZRIatNliwJJc9oED_-r-w=w790-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPkGMqXvqtnpCdLFulOrX7bUca1HFjk6wBReP4jlQjRZw-MX1mC3ZRqnQWLDvbsAOOZdEiughMowNEJ2UQ0Sw7DCEEmeuepzBN0XExntTdu-tltNO65cVXPxaRB67q3k06yGO0QJOQw7yaqqXTcRMBdJw=w791-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczNGFn-scYOIaepHI_TQeJoJrpxwYfd8QC3xOrMBcUv9i5_LZP-r5nhsk8sajKfSmQM5UZHdjfSVCoDUxgxOq08zDnGVgr4qteOgc0AQmAchnM1QB4JZF_9xX6SeFjiFoni3TuU-ZTkVdM-zA2fvMinK9Q=w458-h458-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPFTFK5rdqrMn0nWqIDyrlnH2s3pgKk69kyrr1qqzwjPj6GSURwDWPWu-joIjFgOwKK4V4awyFg8H1iNq73fQfhHz-7_1pjnyrK2yvRSp8__cHyjqNLZLBMd1Mgj0FRey0ZQjKjQYyGE4ojf0s0W4pz6Q=w791-h791-s-no-gm?authuser=0</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/pw/AP1GczPoSEIGxuj78sglLl24PbuEV2k1goSmJlsHJdmAGFgKclRxcX_MzW81pJhR620iy4ifidSqviec2dzAteExySdAq0S0_NpTw0WMzNbkQv4CsQyI_0mzaF3HAUQ5Pou8JB0dUua18YO2OObcPDZ2LxnHoQ=w1200-h791-s-no-gm?authuser=0</t>
   </si>
 </sst>
 </file>
@@ -1628,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,7 +2415,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>157</v>
       </c>
@@ -2435,7 +2450,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>164</v>
       </c>
@@ -2478,7 +2493,7 @@
         <v>172</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>171</v>
+        <v>281</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>173</v>
@@ -2499,10 +2514,10 @@
         <v>12</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>175</v>
       </c>
@@ -2531,7 +2546,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>180</v>
       </c>
@@ -2630,7 +2645,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>198</v>
       </c>
@@ -2662,7 +2677,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>204</v>
       </c>
@@ -2697,7 +2712,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>211</v>
       </c>
@@ -2731,7 +2746,7 @@
         <v>216</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>212</v>
+        <v>277</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>217</v>
@@ -2752,18 +2767,18 @@
         <v>11</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>212</v>
+        <v>277</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>221</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>212</v>
+        <v>278</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>222</v>
@@ -2784,13 +2799,13 @@
         <v>12</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>212</v>
+        <v>278</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>226</v>
       </c>
@@ -2822,7 +2837,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>231</v>
       </c>
@@ -2857,7 +2872,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>238</v>
       </c>
@@ -2889,7 +2904,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>244</v>
       </c>
@@ -2921,12 +2936,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>251</v>
+        <v>279</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>252</v>
@@ -2947,10 +2962,10 @@
         <v>11</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>254</v>
       </c>
@@ -2979,12 +2994,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>258</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>259</v>
@@ -3005,10 +3020,10 @@
         <v>11</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>261</v>
       </c>
@@ -3040,7 +3055,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>266</v>
       </c>
@@ -3072,7 +3087,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>272</v>
       </c>

</xml_diff>